<commit_message>
Add SF Products template and update product modules
Added 'SF Products.xlsx' import template and updated 'Invoice Management.xlsx'. Introduced debug logging in product-modals.js and imported handleImageUpload in products.php. Added product images for ACC004 and updated audit SQL.
</commit_message>
<xml_diff>
--- a/Modular/public/templates/import_files/Invoice Management.xlsx
+++ b/Modular/public/templates/import_files/Invoice Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modular_Software\Modular\public\templates\import_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDC0FBC-CC18-4BD4-A213-F99A42294060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691BD01A-DA02-43A6-B023-275DFF021F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{351F08BE-A637-425E-94E8-B7BFB37B4B97}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{351F08BE-A637-425E-94E8-B7BFB37B4B97}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="3" r:id="rId1"/>
@@ -4319,9 +4319,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000000000"/>
-    <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -4380,7 +4379,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4718,40 +4717,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91AC8F82-48A3-4ED9-A2E7-BA85C64ABBF4}">
   <dimension ref="A1:AB101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R50" sqref="R50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I87" sqref="I87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="33" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.5703125" customWidth="1"/>
-    <col min="21" max="21" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="34" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="59.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="21.85546875" customWidth="1"/>
-    <col min="27" max="27" width="39.140625" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.6328125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="53.6328125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -4837,7 +4839,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -4915,7 +4917,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4993,7 +4995,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -5071,7 +5073,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -5149,7 +5151,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -5227,7 +5229,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -5305,7 +5307,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -5383,7 +5385,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -5461,7 +5463,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -5539,7 +5541,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -5617,7 +5619,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -5695,7 +5697,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -5773,7 +5775,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -5851,7 +5853,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -5929,7 +5931,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -6007,7 +6009,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -6085,7 +6087,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -6163,7 +6165,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -6241,7 +6243,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -6319,7 +6321,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -6397,7 +6399,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -6475,7 +6477,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -6553,7 +6555,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -6631,7 +6633,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -6709,7 +6711,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -6787,7 +6789,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -6865,7 +6867,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -6943,7 +6945,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -7021,7 +7023,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -7099,7 +7101,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -7177,7 +7179,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -7255,7 +7257,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -7333,7 +7335,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -7411,7 +7413,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -7489,7 +7491,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -7567,7 +7569,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -7645,7 +7647,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -7723,7 +7725,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -7801,7 +7803,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -7879,7 +7881,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -7957,7 +7959,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -8035,7 +8037,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -8113,7 +8115,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -8192,7 +8194,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -8270,7 +8272,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -8348,7 +8350,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>15</v>
       </c>
@@ -8426,7 +8428,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -8504,7 +8506,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>15</v>
       </c>
@@ -8585,7 +8587,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -8666,7 +8668,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -8747,7 +8749,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -8828,7 +8830,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>14</v>
       </c>
@@ -8909,7 +8911,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -8990,7 +8992,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -9071,7 +9073,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>14</v>
       </c>
@@ -9152,7 +9154,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>14</v>
       </c>
@@ -9233,7 +9235,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>15</v>
       </c>
@@ -9314,7 +9316,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>15</v>
       </c>
@@ -9396,7 +9398,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -9477,7 +9479,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>15</v>
       </c>
@@ -9558,7 +9560,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>15</v>
       </c>
@@ -9639,7 +9641,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -9720,7 +9722,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>15</v>
       </c>
@@ -9801,7 +9803,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -9882,7 +9884,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>15</v>
       </c>
@@ -9963,7 +9965,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>15</v>
       </c>
@@ -10044,7 +10046,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>15</v>
       </c>
@@ -10125,7 +10127,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>15</v>
       </c>
@@ -10206,7 +10208,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -10287,7 +10289,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -10368,7 +10370,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>15</v>
       </c>
@@ -10449,7 +10451,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>15</v>
       </c>
@@ -10530,7 +10532,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -10611,7 +10613,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -10692,7 +10694,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -10773,7 +10775,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>15</v>
       </c>
@@ -10855,7 +10857,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>14</v>
       </c>
@@ -10936,7 +10938,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>15</v>
       </c>
@@ -11017,7 +11019,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>15</v>
       </c>
@@ -11098,7 +11100,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -11179,7 +11181,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -11260,7 +11262,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -11341,7 +11343,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -11422,7 +11424,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>15</v>
       </c>
@@ -11503,7 +11505,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>15</v>
       </c>
@@ -11585,7 +11587,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -11666,7 +11668,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>14</v>
       </c>
@@ -11747,7 +11749,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>15</v>
       </c>
@@ -11828,7 +11830,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>14</v>
       </c>
@@ -11909,7 +11911,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>14</v>
       </c>
@@ -11990,7 +11992,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>14</v>
       </c>
@@ -12071,7 +12073,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>15</v>
       </c>
@@ -12152,7 +12154,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>14</v>
       </c>
@@ -12233,7 +12235,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>14</v>
       </c>
@@ -12314,7 +12316,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>14</v>
       </c>
@@ -12395,7 +12397,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="97" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>14</v>
       </c>
@@ -12476,7 +12478,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="98" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>14</v>
       </c>
@@ -12557,7 +12559,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="99" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>15</v>
       </c>
@@ -12638,7 +12640,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="100" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>15</v>
       </c>
@@ -12719,7 +12721,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>15</v>
       </c>
@@ -12929,12 +12931,12 @@
       <selection activeCell="A2" sqref="A2:V101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="15" max="15" width="13.5703125" customWidth="1"/>
+    <col min="15" max="15" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -12999,7 +13001,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -13058,7 +13060,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -13114,7 +13116,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -13173,7 +13175,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -13233,7 +13235,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -13292,7 +13294,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -13351,7 +13353,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -13410,7 +13412,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -13469,7 +13471,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -13525,7 +13527,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -13581,7 +13583,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -13641,7 +13643,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -13700,7 +13702,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -13756,7 +13758,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -13812,7 +13814,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -13871,7 +13873,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -13930,7 +13932,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -13986,7 +13988,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -14045,7 +14047,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -14101,7 +14103,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -14157,7 +14159,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -14216,7 +14218,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -14272,7 +14274,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -14331,7 +14333,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -14390,7 +14392,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -14446,7 +14448,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -14505,7 +14507,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -14564,7 +14566,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -14620,7 +14622,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -14676,7 +14678,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -14736,7 +14738,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -14795,7 +14797,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -14854,7 +14856,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -14913,7 +14915,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -14970,7 +14972,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -15029,7 +15031,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -15089,7 +15091,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -15148,7 +15150,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -15207,7 +15209,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -15266,7 +15268,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -15325,7 +15327,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -15381,7 +15383,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -15440,7 +15442,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -15497,7 +15499,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -15556,7 +15558,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -15612,7 +15614,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>15</v>
       </c>
@@ -15671,7 +15673,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -15727,7 +15729,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>15</v>
       </c>
@@ -15783,7 +15785,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -15842,7 +15844,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -15901,7 +15903,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -15961,7 +15963,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>14</v>
       </c>
@@ -16017,7 +16019,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -16077,7 +16079,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -16136,7 +16138,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>14</v>
       </c>
@@ -16195,7 +16197,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>14</v>
       </c>
@@ -16251,7 +16253,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>15</v>
       </c>
@@ -16311,7 +16313,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>15</v>
       </c>
@@ -16371,7 +16373,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -16427,7 +16429,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>15</v>
       </c>
@@ -16483,7 +16485,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>15</v>
       </c>
@@ -16542,7 +16544,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -16601,7 +16603,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>15</v>
       </c>
@@ -16660,7 +16662,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -16719,7 +16721,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>15</v>
       </c>
@@ -16778,7 +16780,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>15</v>
       </c>
@@ -16834,7 +16836,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>15</v>
       </c>
@@ -16893,7 +16895,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>15</v>
       </c>
@@ -16952,7 +16954,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -17011,7 +17013,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -17070,7 +17072,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>15</v>
       </c>
@@ -17126,7 +17128,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>15</v>
       </c>
@@ -17183,7 +17185,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -17242,7 +17244,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -17301,7 +17303,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -17360,7 +17362,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>15</v>
       </c>
@@ -17420,7 +17422,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>14</v>
       </c>
@@ -17479,7 +17481,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>15</v>
       </c>
@@ -17538,7 +17540,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>15</v>
       </c>
@@ -17597,7 +17599,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -17656,7 +17658,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -17715,7 +17717,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -17774,7 +17776,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -17833,7 +17835,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>15</v>
       </c>
@@ -17892,7 +17894,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>15</v>
       </c>
@@ -17952,7 +17954,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -18011,7 +18013,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>14</v>
       </c>
@@ -18070,7 +18072,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>15</v>
       </c>
@@ -18126,7 +18128,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>14</v>
       </c>
@@ -18185,7 +18187,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>14</v>
       </c>
@@ -18241,7 +18243,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>14</v>
       </c>
@@ -18300,7 +18302,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>15</v>
       </c>
@@ -18359,7 +18361,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>14</v>
       </c>
@@ -18419,7 +18421,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>14</v>
       </c>
@@ -18478,7 +18480,7 @@
         <v>1187</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>14</v>
       </c>
@@ -18538,7 +18540,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>14</v>
       </c>
@@ -18597,7 +18599,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>14</v>
       </c>
@@ -18653,7 +18655,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>15</v>
       </c>
@@ -18712,7 +18714,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>15</v>
       </c>
@@ -18771,7 +18773,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>15</v>
       </c>
@@ -18844,14 +18846,14 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>

</xml_diff>